<commit_message>
Update 2020-04-23 part 1
</commit_message>
<xml_diff>
--- a/arkiv-work_default-folders/15KK_nnn_E-15KK_20yy-00nn/repository_operations/maler/N5-kategori-teller-sorter.xlsx
+++ b/arkiv-work_default-folders/15KK_nnn_E-15KK_20yy-00nn/repository_operations/maler/N5-kategori-teller-sorter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arkiv-work\1557\1557_001_E-1557-2018-0001\repository_operations\maler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\arkiv-work\1505\1505_001_E-1505-2018-0001\repository_operations\maler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2EA9BD-57FD-40C4-96E9-F4D959AA288D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2956BE11-6B53-4750-B088-6009BC3B47A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{30DE5284-5CEB-4C0C-910E-E599B308E5D6}"/>
+    <workbookView xWindow="11383" yWindow="2100" windowWidth="20803" windowHeight="15463" activeTab="1" xr2:uid="{30DE5284-5CEB-4C0C-910E-E599B308E5D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tellere kategorisert" sheetId="1" r:id="rId1"/>
@@ -36,34 +36,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Sum hele</t>
-  </si>
-  <si>
-    <t>Snitt hele</t>
-  </si>
-  <si>
     <t>Tatt til etterretning</t>
   </si>
   <si>
-    <t>Besvart med brev</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
     <t>Tatt til orientering</t>
   </si>
   <si>
-    <t xml:space="preserve"> ,Sum 2008-2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ,Snitt 2008-2011</t>
-  </si>
-  <si>
     <t>Sak avsluttet</t>
   </si>
   <si>
     <t>Besvart pr telefon</t>
+  </si>
+  <si>
+    <t>Sum hele:</t>
+  </si>
+  <si>
+    <t>Snitt hele:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,Sum 2008-2011:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,Snitt 2008-2011:</t>
+  </si>
+  <si>
+    <t>Besvart med utgående brev</t>
   </si>
 </sst>
 </file>
@@ -423,101 +423,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52105DA8-49A3-410C-A3D2-3B1B5128EB50}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.140625" style="3"/>
-    <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="3"/>
-    <col min="5" max="16384" width="11.140625" style="1"/>
+    <col min="1" max="2" width="11.15234375" style="3"/>
+    <col min="3" max="3" width="19.3828125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.15234375" style="3"/>
+    <col min="5" max="16384" width="11.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3">
         <f>SUM(B4:B31)</f>
-        <v>10149</v>
+        <v>31165</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3">
+        <f>SUM(B6:B9)</f>
+        <v>31107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="3">
-        <f>SUM(B5:B8)</f>
-        <v>10142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="B2" s="3">
         <f>AVERAGE(B4:B16)</f>
-        <v>1449.8571428571429</v>
+        <v>3462.7777777777778</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3">
-        <f>AVERAGE(B5:B8)</f>
-        <v>2535.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f>AVERAGE(B6:B8)</f>
+        <v>7460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
+        <v>2006</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
         <v>2007</v>
       </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="B5" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
         <v>2008</v>
       </c>
-      <c r="B5" s="3">
-        <v>2409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="B6" s="3">
+        <v>8264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
         <v>2009</v>
       </c>
-      <c r="B6" s="3">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2010</v>
-      </c>
       <c r="B7" s="3">
-        <v>2427</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7911</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>2011</v>
       </c>
       <c r="B8" s="3">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>2013</v>
       </c>
@@ -525,8 +525,24 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>2012</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B12">
     <sortCondition ref="A4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -539,65 +555,65 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="54.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>8869</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1">
-        <v>3543</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
       <c r="B6">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B7">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B6">
+    <sortCondition ref="A1:A6" customList="Besvart med brev,Besvart med e-post,Bevart på telefon,Tatt til etterretning,Tatt til orientering,Besvart med notat,Saken ble avsluttet,NULL"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>